<commit_message>
Adjust cost files relying on US data
</commit_message>
<xml_diff>
--- a/InputData/ccs/CC/CCS Calculations.xlsx
+++ b/InputData/ccs/CC/CCS Calculations.xlsx
@@ -1,16 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="21929"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="5" rupBuild="14420"/>
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\deept\Dropbox\EPS\Input Data for India 2.0\ccs\CC\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Meghan\Documents\eps-india\InputData\ccs\CC\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{03285C26-06C0-4B28-9ED1-5B146403E504}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160"/>
   </bookViews>
   <sheets>
     <sheet name="About" sheetId="1" r:id="rId1"/>
@@ -23,7 +22,7 @@
     <sheet name="CC-TOMCpTS" sheetId="5" r:id="rId8"/>
     <sheet name="CC-EUpTCS" sheetId="6" r:id="rId9"/>
   </sheets>
-  <calcPr calcId="191029"/>
+  <calcPr calcId="162913"/>
   <extLst>
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
       <xcalcf:calcFeatures>
@@ -36,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="151" uniqueCount="116">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="153" uniqueCount="118">
   <si>
     <t>Source:</t>
   </si>
@@ -412,15 +411,21 @@
   <si>
     <t>(Table 6.1)</t>
   </si>
+  <si>
+    <t>India:US cost adjustment</t>
+  </si>
+  <si>
+    <t>see "scaling-factors.xlsx in the InputData folder for source information.</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
   <numFmts count="3">
-    <numFmt numFmtId="164" formatCode="_(&quot;$&quot;* #,##0.00_);_(&quot;$&quot;* \(#,##0.00\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
-    <numFmt numFmtId="165" formatCode="&quot;$&quot;#,##0.00"/>
-    <numFmt numFmtId="171" formatCode="0.000"/>
+    <numFmt numFmtId="44" formatCode="_(&quot;$&quot;* #,##0.00_);_(&quot;$&quot;* \(#,##0.00\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
+    <numFmt numFmtId="164" formatCode="&quot;$&quot;#,##0.00"/>
+    <numFmt numFmtId="165" formatCode="0.000"/>
   </numFmts>
   <fonts count="6" x14ac:knownFonts="1">
     <font>
@@ -627,7 +632,7 @@
   </borders>
   <cellStyleXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="164" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="44" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
   <cellXfs count="48">
@@ -660,10 +665,10 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1"/>
-    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="4" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
@@ -676,14 +681,8 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="171" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
@@ -701,6 +700,12 @@
     </xf>
     <xf numFmtId="2" fontId="0" fillId="4" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
     <xf numFmtId="1" fontId="0" fillId="4" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="3">
     <cellStyle name="Currency" xfId="1" builtinId="4"/>
@@ -933,23 +938,6 @@
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
-        <a:font script="Armn" typeface="Arial"/>
-        <a:font script="Bugi" typeface="Leelawadee UI"/>
-        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
-        <a:font script="Java" typeface="Javanese Text"/>
-        <a:font script="Lisu" typeface="Segoe UI"/>
-        <a:font script="Mymr" typeface="Myanmar Text"/>
-        <a:font script="Nkoo" typeface="Ebrima"/>
-        <a:font script="Olck" typeface="Nirmala UI"/>
-        <a:font script="Osma" typeface="Ebrima"/>
-        <a:font script="Phag" typeface="Phagspa"/>
-        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
-        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
-        <a:font script="Syre" typeface="Estrangelo Edessa"/>
-        <a:font script="Sora" typeface="Nirmala UI"/>
-        <a:font script="Tale" typeface="Microsoft Tai Le"/>
-        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
-        <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
         <a:latin typeface="Calibri" panose="020F0502020204030204"/>
@@ -985,23 +973,6 @@
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
-        <a:font script="Armn" typeface="Arial"/>
-        <a:font script="Bugi" typeface="Leelawadee UI"/>
-        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
-        <a:font script="Java" typeface="Javanese Text"/>
-        <a:font script="Lisu" typeface="Segoe UI"/>
-        <a:font script="Mymr" typeface="Myanmar Text"/>
-        <a:font script="Nkoo" typeface="Ebrima"/>
-        <a:font script="Olck" typeface="Nirmala UI"/>
-        <a:font script="Osma" typeface="Ebrima"/>
-        <a:font script="Phag" typeface="Phagspa"/>
-        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
-        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
-        <a:font script="Syre" typeface="Estrangelo Edessa"/>
-        <a:font script="Sora" typeface="Nirmala UI"/>
-        <a:font script="Tale" typeface="Microsoft Tai Le"/>
-        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
-        <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -1177,34 +1148,36 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D48"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" topLeftCell="A13" workbookViewId="0">
+      <selection activeCell="A44" sqref="A44:A46"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
   <cols>
-    <col min="2" max="2" width="64.42578125" customWidth="1"/>
-    <col min="3" max="3" width="16.7109375" customWidth="1"/>
-    <col min="4" max="4" width="84.42578125" customWidth="1"/>
+    <col min="2" max="2" width="64.3984375" customWidth="1"/>
+    <col min="3" max="3" width="16.73046875" customWidth="1"/>
+    <col min="4" max="4" width="84.3984375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A1" s="27" t="s">
         <v>50</v>
       </c>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A2" s="24" t="s">
         <v>45</v>
       </c>
     </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A3" s="27" t="s">
         <v>46</v>
       </c>
     </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A5" s="1" t="s">
         <v>0</v>
       </c>
@@ -1215,7 +1188,7 @@
         <v>101</v>
       </c>
     </row>
-    <row r="6" spans="1:4" ht="31.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:4" ht="31.5" customHeight="1" x14ac:dyDescent="0.45">
       <c r="B6" s="32" t="s">
         <v>103</v>
       </c>
@@ -1223,7 +1196,7 @@
         <v>65</v>
       </c>
     </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:4" x14ac:dyDescent="0.45">
       <c r="B7" s="31">
         <v>2018</v>
       </c>
@@ -1231,7 +1204,7 @@
         <v>2014</v>
       </c>
     </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:4" x14ac:dyDescent="0.45">
       <c r="B8" t="s">
         <v>104</v>
       </c>
@@ -1239,7 +1212,7 @@
         <v>63</v>
       </c>
     </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:4" x14ac:dyDescent="0.45">
       <c r="B9" t="s">
         <v>105</v>
       </c>
@@ -1247,7 +1220,7 @@
         <v>64</v>
       </c>
     </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:4" x14ac:dyDescent="0.45">
       <c r="B10" t="s">
         <v>106</v>
       </c>
@@ -1255,163 +1228,178 @@
         <v>66</v>
       </c>
     </row>
-    <row r="12" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:4" x14ac:dyDescent="0.45">
       <c r="D12" t="s">
         <v>62</v>
       </c>
     </row>
-    <row r="13" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:4" x14ac:dyDescent="0.45">
       <c r="D13" s="31">
         <v>2010</v>
       </c>
     </row>
-    <row r="14" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:4" x14ac:dyDescent="0.45">
       <c r="D14" t="s">
         <v>61</v>
       </c>
     </row>
-    <row r="15" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:4" x14ac:dyDescent="0.45">
       <c r="D15" s="2" t="s">
         <v>59</v>
       </c>
     </row>
-    <row r="16" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:4" x14ac:dyDescent="0.45">
       <c r="D16" t="s">
         <v>60</v>
       </c>
     </row>
-    <row r="17" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:1" x14ac:dyDescent="0.45">
       <c r="A17" s="1" t="s">
         <v>47</v>
       </c>
     </row>
-    <row r="18" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:1" x14ac:dyDescent="0.45">
       <c r="A18" s="30" t="s">
         <v>56</v>
       </c>
     </row>
-    <row r="19" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:1" x14ac:dyDescent="0.45">
       <c r="A19" s="30" t="s">
         <v>57</v>
       </c>
     </row>
-    <row r="20" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:1" x14ac:dyDescent="0.45">
       <c r="A20" s="30" t="s">
         <v>58</v>
       </c>
     </row>
-    <row r="21" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:1" x14ac:dyDescent="0.45">
       <c r="A21" s="30"/>
     </row>
-    <row r="22" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:1" x14ac:dyDescent="0.45">
       <c r="A22" s="1" t="s">
         <v>87</v>
       </c>
     </row>
-    <row r="23" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:1" x14ac:dyDescent="0.45">
       <c r="A23" s="30" t="s">
         <v>69</v>
       </c>
     </row>
-    <row r="24" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:1" x14ac:dyDescent="0.45">
       <c r="A24" s="30" t="s">
         <v>67</v>
       </c>
     </row>
-    <row r="25" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:1" x14ac:dyDescent="0.45">
       <c r="A25" s="30" t="s">
         <v>68</v>
       </c>
     </row>
-    <row r="26" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:1" x14ac:dyDescent="0.45">
       <c r="A26" s="30"/>
     </row>
-    <row r="27" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:1" x14ac:dyDescent="0.45">
       <c r="A27" s="30" t="s">
         <v>70</v>
       </c>
     </row>
-    <row r="28" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:1" x14ac:dyDescent="0.45">
       <c r="A28" s="30" t="s">
         <v>88</v>
       </c>
     </row>
-    <row r="29" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:1" x14ac:dyDescent="0.45">
       <c r="A29" s="30"/>
     </row>
-    <row r="30" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:1" x14ac:dyDescent="0.45">
       <c r="A30" s="30" t="s">
         <v>89</v>
       </c>
     </row>
-    <row r="31" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:1" x14ac:dyDescent="0.45">
       <c r="A31" s="30" t="s">
         <v>90</v>
       </c>
     </row>
-    <row r="32" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:1" x14ac:dyDescent="0.45">
       <c r="A32" s="30" t="s">
         <v>91</v>
       </c>
     </row>
-    <row r="33" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A33" s="30" t="s">
         <v>92</v>
       </c>
     </row>
-    <row r="34" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A34" s="30" t="s">
         <v>93</v>
       </c>
     </row>
-    <row r="35" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A35" s="30" t="s">
         <v>94</v>
       </c>
     </row>
-    <row r="36" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A36" s="30" t="s">
         <v>98</v>
       </c>
     </row>
-    <row r="37" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A37" s="30" t="s">
         <v>99</v>
       </c>
     </row>
-    <row r="38" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A38" s="30"/>
     </row>
-    <row r="39" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A39" s="30" t="s">
         <v>95</v>
       </c>
     </row>
-    <row r="40" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A40" s="30" t="s">
         <v>96</v>
       </c>
     </row>
-    <row r="41" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A41" s="30" t="s">
         <v>97</v>
       </c>
     </row>
-    <row r="42" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A42" s="30" t="s">
         <v>100</v>
       </c>
     </row>
-    <row r="43" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A43" s="30"/>
     </row>
-    <row r="48" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:2" x14ac:dyDescent="0.45">
+      <c r="A44" t="s">
+        <v>116</v>
+      </c>
+    </row>
+    <row r="45" spans="1:2" x14ac:dyDescent="0.45">
+      <c r="A45" t="s">
+        <v>117</v>
+      </c>
+    </row>
+    <row r="46" spans="1:2" x14ac:dyDescent="0.45">
+      <c r="A46">
+        <v>0.50596615326007366</v>
+      </c>
+    </row>
+    <row r="48" spans="1:2" x14ac:dyDescent="0.45">
       <c r="B48" s="27"/>
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="D9" r:id="rId1" xr:uid="{8874C90D-5C9A-44D6-9C36-0F1BAA7CABAA}"/>
-    <hyperlink ref="D15" r:id="rId2" xr:uid="{AA83E611-79DE-414D-AC06-55715AB9E489}"/>
+    <hyperlink ref="D9" r:id="rId1"/>
+    <hyperlink ref="D15" r:id="rId2"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="1200" verticalDpi="1200" r:id="rId3"/>
@@ -1419,26 +1407,26 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:J37"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
   <cols>
-    <col min="1" max="1" width="31.42578125" customWidth="1"/>
-    <col min="2" max="2" width="10.5703125" customWidth="1"/>
-    <col min="3" max="3" width="11.42578125" customWidth="1"/>
-    <col min="4" max="4" width="9.140625" customWidth="1"/>
+    <col min="1" max="1" width="31.3984375" customWidth="1"/>
+    <col min="2" max="2" width="10.59765625" customWidth="1"/>
+    <col min="3" max="3" width="11.3984375" customWidth="1"/>
+    <col min="4" max="4" width="9.1328125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A1" t="s">
         <v>34</v>
       </c>
     </row>
-    <row r="2" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
-    <row r="3" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:10" ht="14.65" thickBot="1" x14ac:dyDescent="0.5"/>
+    <row r="3" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A3" s="6" t="s">
         <v>3</v>
       </c>
@@ -1461,7 +1449,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="4" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A4" s="9" t="s">
         <v>10</v>
       </c>
@@ -1484,7 +1472,7 @@
         <v>2012</v>
       </c>
     </row>
-    <row r="5" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A5" s="12" t="s">
         <v>1</v>
       </c>
@@ -1498,7 +1486,7 @@
       <c r="I5" s="5"/>
       <c r="J5" s="5"/>
     </row>
-    <row r="6" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A6" s="15" t="s">
         <v>11</v>
       </c>
@@ -1521,7 +1509,7 @@
         <v>525</v>
       </c>
     </row>
-    <row r="7" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A7" s="15" t="s">
         <v>12</v>
       </c>
@@ -1544,7 +1532,7 @@
         <v>2.4</v>
       </c>
     </row>
-    <row r="8" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A8" s="15" t="s">
         <v>13</v>
       </c>
@@ -1567,7 +1555,7 @@
         <v>5677</v>
       </c>
     </row>
-    <row r="9" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A9" s="15" t="s">
         <v>9</v>
       </c>
@@ -1590,7 +1578,7 @@
         <v>829</v>
       </c>
     </row>
-    <row r="10" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A10" s="15" t="s">
         <v>14</v>
       </c>
@@ -1613,7 +1601,7 @@
         <v>4.68</v>
       </c>
     </row>
-    <row r="11" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A11" s="15" t="s">
         <v>15</v>
       </c>
@@ -1636,7 +1624,7 @@
         <v>0.29699999999999999</v>
       </c>
     </row>
-    <row r="12" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A12" s="12" t="s">
         <v>16</v>
       </c>
@@ -1647,7 +1635,7 @@
       <c r="F12" s="18"/>
       <c r="G12" s="19"/>
     </row>
-    <row r="13" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A13" s="15" t="s">
         <v>17</v>
       </c>
@@ -1670,7 +1658,7 @@
         <v>6570</v>
       </c>
     </row>
-    <row r="14" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A14" s="15" t="s">
         <v>18</v>
       </c>
@@ -1693,7 +1681,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="15" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A15" s="15" t="s">
         <v>19</v>
       </c>
@@ -1716,7 +1704,7 @@
         <v>2.93</v>
       </c>
     </row>
-    <row r="16" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A16" s="15" t="s">
         <v>20</v>
       </c>
@@ -1739,7 +1727,7 @@
         <v>90</v>
       </c>
     </row>
-    <row r="17" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A17" s="12" t="s">
         <v>21</v>
       </c>
@@ -1750,7 +1738,7 @@
       <c r="F17" s="18"/>
       <c r="G17" s="19"/>
     </row>
-    <row r="18" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A18" s="15" t="s">
         <v>22</v>
       </c>
@@ -1773,7 +1761,7 @@
         <v>0.33700000000000002</v>
       </c>
     </row>
-    <row r="19" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A19" s="15" t="s">
         <v>23</v>
       </c>
@@ -1796,7 +1784,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="20" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A20" s="15" t="s">
         <v>24</v>
       </c>
@@ -1819,7 +1807,7 @@
         <v>16.600000000000001</v>
       </c>
     </row>
-    <row r="21" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A21" s="15" t="s">
         <v>25</v>
       </c>
@@ -1842,7 +1830,7 @@
         <v>2.4</v>
       </c>
     </row>
-    <row r="22" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A22" s="15" t="s">
         <v>26</v>
       </c>
@@ -1865,7 +1853,7 @@
         <v>3.1</v>
       </c>
     </row>
-    <row r="23" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A23" s="15" t="s">
         <v>27</v>
       </c>
@@ -1888,7 +1876,7 @@
         <v>60.1</v>
       </c>
     </row>
-    <row r="24" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A24" s="12" t="s">
         <v>28</v>
       </c>
@@ -1899,7 +1887,7 @@
       <c r="F24" s="18"/>
       <c r="G24" s="19"/>
     </row>
-    <row r="25" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A25" s="15" t="s">
         <v>29</v>
       </c>
@@ -1922,7 +1910,7 @@
         <v>90</v>
       </c>
     </row>
-    <row r="26" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A26" s="15" t="s">
         <v>13</v>
       </c>
@@ -1945,7 +1933,7 @@
         <v>6308</v>
       </c>
     </row>
-    <row r="27" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A27" s="15" t="s">
         <v>11</v>
       </c>
@@ -1968,7 +1956,7 @@
         <v>894</v>
       </c>
     </row>
-    <row r="28" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A28" s="15" t="s">
         <v>22</v>
       </c>
@@ -1991,7 +1979,7 @@
         <v>3.6999999999999998E-2</v>
       </c>
     </row>
-    <row r="29" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A29" s="15" t="s">
         <v>23</v>
       </c>
@@ -2014,7 +2002,7 @@
         <v>20.399999999999999</v>
       </c>
     </row>
-    <row r="30" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A30" s="15" t="s">
         <v>24</v>
       </c>
@@ -2037,7 +2025,7 @@
         <v>18.5</v>
       </c>
     </row>
-    <row r="31" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A31" s="15" t="s">
         <v>25</v>
       </c>
@@ -2060,7 +2048,7 @@
         <v>4.4000000000000004</v>
       </c>
     </row>
-    <row r="32" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A32" s="15" t="s">
         <v>26</v>
       </c>
@@ -2083,7 +2071,7 @@
         <v>4.33</v>
       </c>
     </row>
-    <row r="33" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A33" s="15" t="s">
         <v>27</v>
       </c>
@@ -2106,7 +2094,7 @@
         <v>54.1</v>
       </c>
     </row>
-    <row r="34" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A34" s="12" t="s">
         <v>30</v>
       </c>
@@ -2117,7 +2105,7 @@
       <c r="F34" s="18"/>
       <c r="G34" s="19"/>
     </row>
-    <row r="35" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A35" s="15" t="s">
         <v>31</v>
       </c>
@@ -2140,7 +2128,7 @@
         <v>1.23</v>
       </c>
     </row>
-    <row r="36" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A36" s="15" t="s">
         <v>32</v>
       </c>
@@ -2163,7 +2151,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="37" spans="1:7" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="37" spans="1:7" ht="28.9" thickBot="1" x14ac:dyDescent="0.5">
       <c r="A37" s="20" t="s">
         <v>33</v>
       </c>
@@ -2192,28 +2180,28 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:C22"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A17" sqref="A17:C22"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
   <cols>
-    <col min="1" max="1" width="17.5703125" customWidth="1"/>
-    <col min="2" max="2" width="20.28515625" customWidth="1"/>
-    <col min="3" max="3" width="19.42578125" customWidth="1"/>
+    <col min="1" max="1" width="17.59765625" customWidth="1"/>
+    <col min="2" max="2" width="20.265625" customWidth="1"/>
+    <col min="3" max="3" width="19.3984375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A1" s="25" t="s">
         <v>52</v>
       </c>
       <c r="B1" s="4"/>
       <c r="C1" s="4"/>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A2" s="1"/>
       <c r="B2" s="1" t="s">
         <v>36</v>
@@ -2222,7 +2210,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A3" s="1" t="s">
         <v>2</v>
       </c>
@@ -2235,7 +2223,7 @@
         <v>829</v>
       </c>
     </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A4" s="1" t="s">
         <v>37</v>
       </c>
@@ -2248,7 +2236,7 @@
         <v>6570</v>
       </c>
     </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A5" s="1" t="s">
         <v>38</v>
       </c>
@@ -2259,7 +2247,7 @@
         <v>1000</v>
       </c>
     </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A6" s="1" t="s">
         <v>39</v>
       </c>
@@ -2272,19 +2260,19 @@
         <v>126.17960426179603</v>
       </c>
     </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A7" s="1"/>
       <c r="B7" s="23"/>
       <c r="C7" s="23"/>
     </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A9" s="25" t="s">
         <v>40</v>
       </c>
       <c r="B9" s="4"/>
       <c r="C9" s="4"/>
     </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A10" s="1"/>
       <c r="B10" s="1" t="s">
         <v>36</v>
@@ -2293,7 +2281,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="11" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A11" s="1" t="s">
         <v>7</v>
       </c>
@@ -2306,7 +2294,7 @@
         <v>4.68</v>
       </c>
     </row>
-    <row r="12" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A12" s="1" t="s">
         <v>41</v>
       </c>
@@ -2317,7 +2305,7 @@
         <v>1E-3</v>
       </c>
     </row>
-    <row r="13" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A13" s="1" t="s">
         <v>38</v>
       </c>
@@ -2328,7 +2316,7 @@
         <v>1000</v>
       </c>
     </row>
-    <row r="14" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A14" s="1" t="s">
         <v>54</v>
       </c>
@@ -2341,14 +2329,14 @@
         <v>4.68</v>
       </c>
     </row>
-    <row r="17" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A17" s="3" t="s">
         <v>42</v>
       </c>
       <c r="B17" s="4"/>
       <c r="C17" s="4"/>
     </row>
-    <row r="18" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:3" x14ac:dyDescent="0.45">
       <c r="B18" s="1" t="s">
         <v>36</v>
       </c>
@@ -2356,7 +2344,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="19" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A19" s="1" t="s">
         <v>8</v>
       </c>
@@ -2369,7 +2357,7 @@
         <v>0.29699999999999999</v>
       </c>
     </row>
-    <row r="20" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A20" s="1" t="s">
         <v>38</v>
       </c>
@@ -2380,7 +2368,7 @@
         <v>1000</v>
       </c>
     </row>
-    <row r="21" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A21" s="1" t="s">
         <v>43</v>
       </c>
@@ -2391,7 +2379,7 @@
         <v>3412</v>
       </c>
     </row>
-    <row r="22" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A22" s="1" t="s">
         <v>44</v>
       </c>
@@ -2410,44 +2398,44 @@
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{32EF6D6A-CAEA-4466-8367-59ADEEC6827B}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:B6"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="E8" sqref="E8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
   <cols>
     <col min="1" max="1" width="18" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="36.42578125" customWidth="1"/>
+    <col min="2" max="2" width="36.3984375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A1" s="43" t="s">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.45">
+      <c r="A1" s="41" t="s">
         <v>107</v>
       </c>
-      <c r="B1" s="44" t="s">
+      <c r="B1" s="42" t="s">
         <v>108</v>
       </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A2" s="42">
+    <row r="2" spans="1:2" x14ac:dyDescent="0.45">
+      <c r="A2" s="40">
         <v>2016</v>
       </c>
-      <c r="B2" s="42">
+      <c r="B2" s="40">
         <v>67.95</v>
       </c>
     </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A4" t="s">
         <v>111</v>
       </c>
-      <c r="B4" s="44" t="s">
+      <c r="B4" s="42" t="s">
         <v>112</v>
       </c>
     </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A5" t="s">
         <v>109</v>
       </c>
@@ -2455,7 +2443,7 @@
         <v>110</v>
       </c>
     </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A6">
         <v>2016</v>
       </c>
@@ -2469,14 +2457,14 @@
 </file>
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A21A2C14-1D85-4685-938F-DAD9ED607BBB}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="H8" sqref="H8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <drawing r:id="rId1"/>
@@ -2484,25 +2472,25 @@
 </file>
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5E80723D-912F-4B6D-BFE2-2D7E8918B54C}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:H21"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="B3" sqref="B3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
   <cols>
-    <col min="1" max="1" width="36.42578125" customWidth="1"/>
-    <col min="2" max="2" width="20.28515625" customWidth="1"/>
+    <col min="1" max="1" width="36.3984375" customWidth="1"/>
+    <col min="2" max="2" width="20.265625" customWidth="1"/>
     <col min="3" max="3" width="22" customWidth="1"/>
-    <col min="4" max="4" width="16.7109375" customWidth="1"/>
-    <col min="6" max="6" width="24.42578125" customWidth="1"/>
-    <col min="7" max="7" width="11.28515625" customWidth="1"/>
+    <col min="4" max="4" width="16.73046875" customWidth="1"/>
+    <col min="6" max="6" width="24.3984375" customWidth="1"/>
+    <col min="7" max="7" width="11.265625" customWidth="1"/>
     <col min="8" max="8" width="11" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A1" s="3" t="s">
         <v>76</v>
       </c>
@@ -2510,52 +2498,52 @@
       <c r="C1" s="3"/>
       <c r="D1" s="3"/>
     </row>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="B2" s="35" t="s">
+    <row r="2" spans="1:8" x14ac:dyDescent="0.45">
+      <c r="B2" s="46" t="s">
         <v>73</v>
       </c>
-      <c r="C2" s="36"/>
-    </row>
-    <row r="3" spans="1:8" ht="30" x14ac:dyDescent="0.25">
-      <c r="B3" s="37" t="s">
+      <c r="C2" s="47"/>
+    </row>
+    <row r="3" spans="1:8" ht="28.5" x14ac:dyDescent="0.45">
+      <c r="B3" s="35" t="s">
         <v>71</v>
       </c>
-      <c r="C3" s="37" t="s">
+      <c r="C3" s="35" t="s">
         <v>72</v>
       </c>
-      <c r="F3" s="41" t="s">
+      <c r="F3" s="39" t="s">
         <v>85</v>
       </c>
-      <c r="G3" s="38">
+      <c r="G3" s="36">
         <f>AVERAGE(1.06, 1.16)</f>
         <v>1.1099999999999999</v>
       </c>
-      <c r="H3" s="40" t="s">
+      <c r="H3" s="38" t="s">
         <v>115</v>
       </c>
     </row>
-    <row r="4" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A4" s="38" t="s">
+    <row r="4" spans="1:8" x14ac:dyDescent="0.45">
+      <c r="A4" s="36" t="s">
         <v>77</v>
       </c>
-      <c r="B4" s="38">
+      <c r="B4" s="36">
         <f>19*10^7</f>
         <v>190000000</v>
       </c>
-      <c r="C4" s="38">
+      <c r="C4" s="36">
         <f>23*10^7</f>
         <v>230000000</v>
       </c>
     </row>
-    <row r="5" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A5" s="38" t="s">
+    <row r="5" spans="1:8" x14ac:dyDescent="0.45">
+      <c r="A5" s="36" t="s">
         <v>78</v>
       </c>
-      <c r="B5" s="38">
+      <c r="B5" s="36">
         <f>246*10^5</f>
         <v>24600000</v>
       </c>
-      <c r="C5" s="38">
+      <c r="C5" s="36">
         <f>221*10^5</f>
         <v>22100000</v>
       </c>
@@ -2564,24 +2552,24 @@
       </c>
       <c r="G5" s="4"/>
     </row>
-    <row r="6" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A6" s="38" t="s">
+    <row r="6" spans="1:8" x14ac:dyDescent="0.45">
+      <c r="A6" s="36" t="s">
         <v>74</v>
       </c>
-      <c r="B6" s="38">
+      <c r="B6" s="36">
         <v>3736.04</v>
       </c>
-      <c r="C6" s="38">
+      <c r="C6" s="36">
         <v>3966.02</v>
       </c>
-      <c r="D6" s="40" t="s">
+      <c r="D6" s="38" t="s">
         <v>84</v>
       </c>
-      <c r="G6" s="45" t="s">
+      <c r="G6" s="43" t="s">
         <v>86</v>
       </c>
     </row>
-    <row r="7" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:8" x14ac:dyDescent="0.45">
       <c r="F7" s="1" t="s">
         <v>8</v>
       </c>
@@ -2590,7 +2578,7 @@
         <v>0.90090090090090102</v>
       </c>
     </row>
-    <row r="8" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A8" s="1" t="s">
         <v>75</v>
       </c>
@@ -2602,11 +2590,11 @@
       </c>
       <c r="H8" s="5"/>
     </row>
-    <row r="9" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A9" s="38" t="s">
+    <row r="9" spans="1:8" x14ac:dyDescent="0.45">
+      <c r="A9" s="36" t="s">
         <v>77</v>
       </c>
-      <c r="B9" s="38">
+      <c r="B9" s="36">
         <f>AVERAGE(B4:C4)</f>
         <v>210000000</v>
       </c>
@@ -2618,45 +2606,45 @@
       </c>
       <c r="H9" s="1"/>
     </row>
-    <row r="10" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A10" s="38" t="s">
+    <row r="10" spans="1:8" x14ac:dyDescent="0.45">
+      <c r="A10" s="36" t="s">
         <v>79</v>
       </c>
-      <c r="B10" s="38">
+      <c r="B10" s="36">
         <f>AVERAGE(B5:C5)</f>
         <v>23350000</v>
       </c>
       <c r="F10" s="1" t="s">
         <v>44</v>
       </c>
-      <c r="G10" s="47">
+      <c r="G10" s="45">
         <f>G7*G8*G9</f>
         <v>3073873.8738738741</v>
       </c>
     </row>
-    <row r="11" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A11" s="38" t="s">
+    <row r="11" spans="1:8" x14ac:dyDescent="0.45">
+      <c r="A11" s="36" t="s">
         <v>74</v>
       </c>
-      <c r="B11" s="38">
+      <c r="B11" s="36">
         <f t="shared" ref="B11" si="0">AVERAGE(B6:C6)</f>
         <v>3851.0299999999997</v>
       </c>
     </row>
-    <row r="13" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A13" s="38" t="s">
+    <row r="13" spans="1:8" x14ac:dyDescent="0.45">
+      <c r="A13" s="36" t="s">
         <v>80</v>
       </c>
-      <c r="B13" s="39">
+      <c r="B13" s="37">
         <f>B10/B9</f>
         <v>0.11119047619047619</v>
       </c>
     </row>
-    <row r="14" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A14" s="38" t="s">
+    <row r="14" spans="1:8" x14ac:dyDescent="0.45">
+      <c r="A14" s="36" t="s">
         <v>81</v>
       </c>
-      <c r="B14" s="39">
+      <c r="B14" s="37">
         <f>B13*B11</f>
         <v>428.19785952380948</v>
       </c>
@@ -2664,16 +2652,16 @@
         <v>83</v>
       </c>
     </row>
-    <row r="15" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A15" s="38" t="s">
+    <row r="15" spans="1:8" x14ac:dyDescent="0.45">
+      <c r="A15" s="36" t="s">
         <v>82</v>
       </c>
-      <c r="B15" s="39">
+      <c r="B15" s="37">
         <f>B11-B14</f>
         <v>3422.83214047619</v>
       </c>
     </row>
-    <row r="17" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:3" x14ac:dyDescent="0.45">
       <c r="B17" s="28">
         <f>B14/'Conversion Factors'!B2</f>
         <v>6.3016609201443634</v>
@@ -2682,11 +2670,11 @@
         <v>113</v>
       </c>
     </row>
-    <row r="18" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A18" s="38" t="s">
+    <row r="18" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="A18" s="36" t="s">
         <v>81</v>
       </c>
-      <c r="B18" s="46">
+      <c r="B18" s="44">
         <f>B17*'Conversion Factors'!B6</f>
         <v>6.0282555812939824</v>
       </c>
@@ -2694,7 +2682,7 @@
         <v>114</v>
       </c>
     </row>
-    <row r="20" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:3" x14ac:dyDescent="0.45">
       <c r="B20" s="28">
         <f>B15/'Conversion Factors'!B2</f>
         <v>50.37280559935526</v>
@@ -2703,11 +2691,11 @@
         <v>113</v>
       </c>
     </row>
-    <row r="21" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A21" s="38" t="s">
+    <row r="21" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="A21" s="36" t="s">
         <v>82</v>
       </c>
-      <c r="B21" s="46">
+      <c r="B21" s="44">
         <f>B20*'Conversion Factors'!B6</f>
         <v>48.187319239765387</v>
       </c>
@@ -2725,7 +2713,103 @@
 </file>
 
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <sheetPr>
+    <tabColor theme="3"/>
+  </sheetPr>
+  <dimension ref="A1:B3"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B3" sqref="B3"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
+  <cols>
+    <col min="1" max="1" width="56.1328125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="24.59765625" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:2" x14ac:dyDescent="0.45">
+      <c r="A1" s="27" t="s">
+        <v>50</v>
+      </c>
+      <c r="B1" s="29" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.45">
+      <c r="A2" t="s">
+        <v>48</v>
+      </c>
+      <c r="B2" s="28">
+        <f>Calcs!B21*About!$A$46</f>
+        <v>24.38115255165923</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.45">
+      <c r="A3" t="s">
+        <v>49</v>
+      </c>
+      <c r="B3" s="28">
+        <f>B2</f>
+        <v>24.38115255165923</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <sheetPr>
+    <tabColor theme="3"/>
+  </sheetPr>
+  <dimension ref="A1:B3"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B3" sqref="B3"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
+  <cols>
+    <col min="1" max="1" width="43.1328125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="25.86328125" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:2" x14ac:dyDescent="0.45">
+      <c r="A1" s="24" t="s">
+        <v>45</v>
+      </c>
+      <c r="B1" s="29" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.45">
+      <c r="A2" t="s">
+        <v>48</v>
+      </c>
+      <c r="B2" s="28">
+        <f>Calcs!B18*About!$A$46</f>
+        <v>3.0500932873358857</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.45">
+      <c r="A3" t="s">
+        <v>49</v>
+      </c>
+      <c r="B3" s="28">
+        <f>B2</f>
+        <v>3.0500932873358857</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr>
     <tabColor theme="3"/>
   </sheetPr>
@@ -2735,109 +2819,13 @@
       <selection activeCell="B4" sqref="B4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
   <cols>
-    <col min="1" max="1" width="56.140625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="24.5703125" customWidth="1"/>
+    <col min="1" max="1" width="37.265625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="42.59765625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A1" s="27" t="s">
-        <v>50</v>
-      </c>
-      <c r="B1" s="29" t="s">
-        <v>51</v>
-      </c>
-    </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A2" t="s">
-        <v>48</v>
-      </c>
-      <c r="B2" s="28">
-        <f>Calcs!B21</f>
-        <v>48.187319239765387</v>
-      </c>
-    </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A3" t="s">
-        <v>49</v>
-      </c>
-      <c r="B3" s="28">
-        <f>B2</f>
-        <v>48.187319239765387</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0400-000000000000}">
-  <sheetPr>
-    <tabColor theme="3"/>
-  </sheetPr>
-  <dimension ref="A1:B3"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B4" sqref="B4"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <cols>
-    <col min="1" max="1" width="43.140625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="25.85546875" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A1" s="24" t="s">
-        <v>45</v>
-      </c>
-      <c r="B1" s="29" t="s">
-        <v>53</v>
-      </c>
-    </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A2" t="s">
-        <v>48</v>
-      </c>
-      <c r="B2" s="28">
-        <f>Calcs!B18</f>
-        <v>6.0282555812939824</v>
-      </c>
-    </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A3" t="s">
-        <v>49</v>
-      </c>
-      <c r="B3" s="28">
-        <f>B2</f>
-        <v>6.0282555812939824</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0500-000000000000}">
-  <sheetPr>
-    <tabColor theme="3"/>
-  </sheetPr>
-  <dimension ref="A1:B3"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B4" sqref="B4"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <cols>
-    <col min="1" max="1" width="37.28515625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="42.5703125" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A1" s="27" t="s">
         <v>46</v>
       </c>
@@ -2845,7 +2833,7 @@
         <v>55</v>
       </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A2" t="s">
         <v>48</v>
       </c>
@@ -2854,7 +2842,7 @@
         <v>3073873.8738738741</v>
       </c>
     </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A3" t="s">
         <v>49</v>
       </c>

</xml_diff>